<commit_message>
completed registrar master and registrar master branches excel upload
</commit_message>
<xml_diff>
--- a/public/Sample_Registrar_Masters.xlsx
+++ b/public/Sample_Registrar_Masters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Registrar Name*</t>
   </si>
@@ -19,77 +19,17 @@
     <t>SEBI Regn. ID*</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Pincode</t>
-  </si>
-  <si>
-    <t>Telephone 1</t>
-  </si>
-  <si>
-    <t>Telephone 2</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Name of Contact Person</t>
-  </si>
-  <si>
-    <t>Designation of Contact Person</t>
-  </si>
-  <si>
-    <t>Email of Contact Person</t>
-  </si>
-  <si>
-    <t>Phone of Contact Person</t>
-  </si>
-  <si>
-    <t>Officer Assigned</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>Company Master Id*</t>
-  </si>
-  <si>
     <t>KFIN Technologies Private Limited</t>
   </si>
   <si>
     <t>INR000000221</t>
   </si>
-  <si>
-    <t>6TH CROSS</t>
-  </si>
-  <si>
-    <t>BENGALURU</t>
-  </si>
-  <si>
-    <t>Karnataka</t>
-  </si>
-  <si>
-    <t>SAHASUBHAM043@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>OM SAI</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -97,15 +37,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="8.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,22 +50,8 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF888888"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF888888"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF888888"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF888888"/>
-      </bottom>
-    </border>
     <border>
       <left style="thin">
         <color rgb="FF757575"/>
@@ -150,24 +70,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,98 +300,14 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1">
-        <v>560076.0</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>